<commit_message>
Fix execution error in 2_ET_20201
</commit_message>
<xml_diff>
--- a/2_ET_20201/Specifications/Specification_Advanced.xlsx
+++ b/2_ET_20201/Specifications/Specification_Advanced.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="43">
   <si>
     <t>TEST CASE ID</t>
   </si>
@@ -154,9 +154,6 @@
   </si>
   <si>
     <t xml:space="preserve">EV_HV_02 </t>
-  </si>
-  <si>
-    <t>StateOfCharge sinks slower than 0.1% of fully charged level in 5s</t>
   </si>
 </sst>
 </file>
@@ -899,7 +896,7 @@
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1024,7 +1021,7 @@
       <c r="A16" s="30"/>
       <c r="B16" s="10"/>
       <c r="C16" s="11" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -1446,6 +1443,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101000803C505E8A4754993AF39679BCFD47A" ma:contentTypeVersion="0" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="0bcaa11129a0f47130266f866b106bcb">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b4f5dc90cf06628c3b90945c8266c24d">
     <xsd:element name="properties">
@@ -1559,12 +1562,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9A73F463-E313-4D89-A3F0-1856B93F4AD7}">
   <ds:schemaRefs>
@@ -1574,6 +1571,21 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3DD1D562-F9D5-48FA-9E4D-E0F2968F8454}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{86E26950-EC73-4E81-8E7F-C6B4258F5870}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1587,19 +1599,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3DD1D562-F9D5-48FA-9E4D-E0F2968F8454}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>